<commit_message>
2nd Algorithm Part Done
2nd Algorithm assigns best sort to projects. Distributes to ensure all projects have at least min amount of members.
</commit_message>
<xml_diff>
--- a/Samples/CSVs/Fall_2022_Edit_1.05_Students.xlsx
+++ b/Samples/CSVs/Fall_2022_Edit_1.05_Students.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Christopher\UT-Student-Assignment\Samples\CSVs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E0C4E19-46A7-46A3-A112-2587529990E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AEF5284-9743-4508-8089-57D955E9D993}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Student_Info" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="266">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="270">
   <si>
     <t>Name</t>
   </si>
@@ -835,6 +835,18 @@
   </si>
   <si>
     <t>I20</t>
+  </si>
+  <si>
+    <t>Name100</t>
+  </si>
+  <si>
+    <t>EID100</t>
+  </si>
+  <si>
+    <t>Name101</t>
+  </si>
+  <si>
+    <t>EID101</t>
   </si>
 </sst>
 </file>
@@ -1152,10 +1164,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AQ100"/>
+  <dimension ref="A1:AQ102"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="J67" sqref="J67"/>
+    <sheetView tabSelected="1" topLeftCell="A93" workbookViewId="0">
+      <selection activeCell="AS96" sqref="AS96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1791,13 +1803,13 @@
         <v>4</v>
       </c>
       <c r="AM5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AO5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AP5">
         <v>3</v>
@@ -14117,6 +14129,268 @@
       </c>
       <c r="AQ100">
         <v>2</v>
+      </c>
+    </row>
+    <row r="101" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>266</v>
+      </c>
+      <c r="B101" t="s">
+        <v>267</v>
+      </c>
+      <c r="C101">
+        <v>3.3</v>
+      </c>
+      <c r="D101">
+        <v>0</v>
+      </c>
+      <c r="E101">
+        <v>0</v>
+      </c>
+      <c r="F101">
+        <v>1</v>
+      </c>
+      <c r="G101">
+        <v>0</v>
+      </c>
+      <c r="H101">
+        <v>0</v>
+      </c>
+      <c r="I101" t="s">
+        <v>126</v>
+      </c>
+      <c r="J101">
+        <v>2</v>
+      </c>
+      <c r="K101">
+        <v>4</v>
+      </c>
+      <c r="L101">
+        <v>2</v>
+      </c>
+      <c r="M101">
+        <v>1</v>
+      </c>
+      <c r="N101">
+        <v>1</v>
+      </c>
+      <c r="O101">
+        <v>1</v>
+      </c>
+      <c r="P101">
+        <v>4</v>
+      </c>
+      <c r="Q101">
+        <v>4</v>
+      </c>
+      <c r="R101">
+        <v>1</v>
+      </c>
+      <c r="S101">
+        <v>4</v>
+      </c>
+      <c r="T101">
+        <v>5</v>
+      </c>
+      <c r="U101">
+        <v>3</v>
+      </c>
+      <c r="V101">
+        <v>4</v>
+      </c>
+      <c r="W101">
+        <v>5</v>
+      </c>
+      <c r="X101">
+        <v>5</v>
+      </c>
+      <c r="Y101">
+        <v>4</v>
+      </c>
+      <c r="Z101">
+        <v>5</v>
+      </c>
+      <c r="AA101">
+        <v>5</v>
+      </c>
+      <c r="AB101">
+        <v>2</v>
+      </c>
+      <c r="AC101">
+        <v>3</v>
+      </c>
+      <c r="AD101">
+        <v>1</v>
+      </c>
+      <c r="AE101">
+        <v>2</v>
+      </c>
+      <c r="AF101">
+        <v>3</v>
+      </c>
+      <c r="AG101">
+        <v>1</v>
+      </c>
+      <c r="AH101">
+        <v>4</v>
+      </c>
+      <c r="AI101">
+        <v>2</v>
+      </c>
+      <c r="AJ101">
+        <v>1</v>
+      </c>
+      <c r="AK101">
+        <v>2</v>
+      </c>
+      <c r="AL101">
+        <v>3</v>
+      </c>
+      <c r="AM101">
+        <v>2</v>
+      </c>
+      <c r="AN101">
+        <v>1</v>
+      </c>
+      <c r="AO101">
+        <v>3</v>
+      </c>
+      <c r="AP101">
+        <v>1</v>
+      </c>
+      <c r="AQ101">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="102" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>268</v>
+      </c>
+      <c r="B102" t="s">
+        <v>269</v>
+      </c>
+      <c r="C102">
+        <v>3.7</v>
+      </c>
+      <c r="D102">
+        <v>1</v>
+      </c>
+      <c r="E102">
+        <v>1</v>
+      </c>
+      <c r="F102">
+        <v>0</v>
+      </c>
+      <c r="G102">
+        <v>0</v>
+      </c>
+      <c r="H102">
+        <v>0</v>
+      </c>
+      <c r="I102" t="s">
+        <v>234</v>
+      </c>
+      <c r="J102">
+        <v>1</v>
+      </c>
+      <c r="K102">
+        <v>1</v>
+      </c>
+      <c r="L102">
+        <v>1</v>
+      </c>
+      <c r="M102">
+        <v>1</v>
+      </c>
+      <c r="N102">
+        <v>1</v>
+      </c>
+      <c r="O102">
+        <v>1</v>
+      </c>
+      <c r="P102">
+        <v>1</v>
+      </c>
+      <c r="Q102">
+        <v>1</v>
+      </c>
+      <c r="R102">
+        <v>5</v>
+      </c>
+      <c r="S102">
+        <v>1</v>
+      </c>
+      <c r="T102">
+        <v>1</v>
+      </c>
+      <c r="U102">
+        <v>1</v>
+      </c>
+      <c r="V102">
+        <v>5</v>
+      </c>
+      <c r="W102">
+        <v>4</v>
+      </c>
+      <c r="X102">
+        <v>2</v>
+      </c>
+      <c r="Y102">
+        <v>3</v>
+      </c>
+      <c r="Z102">
+        <v>3</v>
+      </c>
+      <c r="AA102">
+        <v>4</v>
+      </c>
+      <c r="AB102">
+        <v>2</v>
+      </c>
+      <c r="AC102">
+        <v>4</v>
+      </c>
+      <c r="AD102">
+        <v>3</v>
+      </c>
+      <c r="AE102">
+        <v>1</v>
+      </c>
+      <c r="AF102">
+        <v>5</v>
+      </c>
+      <c r="AG102">
+        <v>3</v>
+      </c>
+      <c r="AH102">
+        <v>2</v>
+      </c>
+      <c r="AI102">
+        <v>1</v>
+      </c>
+      <c r="AJ102">
+        <v>4</v>
+      </c>
+      <c r="AK102">
+        <v>5</v>
+      </c>
+      <c r="AL102">
+        <v>2</v>
+      </c>
+      <c r="AM102">
+        <v>3</v>
+      </c>
+      <c r="AN102">
+        <v>4</v>
+      </c>
+      <c r="AO102">
+        <v>2</v>
+      </c>
+      <c r="AP102">
+        <v>1</v>
+      </c>
+      <c r="AQ102">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -14128,7 +14402,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C824E7E0-FD0D-402F-9FBD-7A8EB607EF1A}">
   <dimension ref="A1:Z100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="T1" sqref="T1"/>
     </sheetView>
   </sheetViews>

</xml_diff>